<commit_message>
updated code on 27/03/2024
</commit_message>
<xml_diff>
--- a/backend/testportal/media/excel/res.xlsx
+++ b/backend/testportal/media/excel/res.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,69 +500,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Yashraj</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>WCE</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CSE</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>yashraj_s_patil@whirlpool.com</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>B.Tech</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>9876543210</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Computer Science/Information Technology</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>M.Tech</t>
-        </is>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>3</v>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>http://127.0.0.1:8000/media/resume/IGN13_NovoSconceAutoRegTesting_Heyer.pdf</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>